<commit_message>
moving old to new file
</commit_message>
<xml_diff>
--- a/cse-seminars/cse-seminars-roster.xlsx
+++ b/cse-seminars/cse-seminars-roster.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="old" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" dpi="72" codePage="10000"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>Mike Bain</t>
   </si>
@@ -71,15 +70,9 @@
     <t>Manuel Chakravarty</t>
   </si>
   <si>
-    <t>Lijun Chang</t>
-  </si>
-  <si>
     <t>ARC DECRA Fellow</t>
   </si>
   <si>
-    <t>Chun Tung Chou</t>
-  </si>
-  <si>
     <t>Peng Di</t>
   </si>
   <si>
@@ -104,21 +97,6 @@
     <t>Senior Lecturer &amp; Program Director - Bioinformatics</t>
   </si>
   <si>
-    <t>Serge Gaspers</t>
-  </si>
-  <si>
-    <t>Senior Lecturer &amp; ARC Future Fellow</t>
-  </si>
-  <si>
-    <t>Hui Annie Guo</t>
-  </si>
-  <si>
-    <t>Senior Lecturer &amp; Program Director - Computer Engineering</t>
-  </si>
-  <si>
-    <t>Mahbub Hassan</t>
-  </si>
-  <si>
     <t>Professor</t>
   </si>
   <si>
@@ -137,9 +115,6 @@
     <t>Senior Research Associate (Level B)</t>
   </si>
   <si>
-    <t>Wen Hu</t>
-  </si>
-  <si>
     <t>Zengfeng Huang</t>
   </si>
   <si>
@@ -149,12 +124,6 @@
     <t>Aleksandar Ignjatovic</t>
   </si>
   <si>
-    <t>Sanjay Jha</t>
-  </si>
-  <si>
-    <t>Salil Kanhere</t>
-  </si>
-  <si>
     <t>Gabriele Keller</t>
   </si>
   <si>
@@ -170,9 +139,6 @@
     <t>Chengwen Luo</t>
   </si>
   <si>
-    <t>Nadine Marcus</t>
-  </si>
-  <si>
     <t>Eric Martin</t>
   </si>
   <si>
@@ -185,12 +151,6 @@
     <t>Eilish O'rourke</t>
   </si>
   <si>
-    <t>Maurice Pagnucco</t>
-  </si>
-  <si>
-    <t>Professor &amp; Head of School</t>
-  </si>
-  <si>
     <t>Helen Hye-Young Paik</t>
   </si>
   <si>
@@ -203,18 +163,9 @@
     <t>Professor &amp; Postgraduate Research and Scholarship Co-ordinator</t>
   </si>
   <si>
-    <t>Jorgen Peddersen</t>
-  </si>
-  <si>
     <t>Jianbin Qin</t>
   </si>
   <si>
-    <t>Fethi Rabhi</t>
-  </si>
-  <si>
-    <t>Professor &amp; Program Director - Software Engineering</t>
-  </si>
-  <si>
     <t>David Rajaratnam</t>
   </si>
   <si>
@@ -224,12 +175,6 @@
     <t>Abdallah Saffidine</t>
   </si>
   <si>
-    <t>Claude Sammut</t>
-  </si>
-  <si>
-    <t>Professor &amp; Research Committee Chair</t>
-  </si>
-  <si>
     <t>John Shepherd</t>
   </si>
   <si>
@@ -248,9 +193,6 @@
     <t>Andrew Taylor</t>
   </si>
   <si>
-    <t>Michael Thielscher</t>
-  </si>
-  <si>
     <t>Ron Van Der Meyden</t>
   </si>
   <si>
@@ -260,12 +202,6 @@
     <t>Nicta Chair in Artificial Intelligence &amp; Professor</t>
   </si>
   <si>
-    <t>Wei Wang</t>
-  </si>
-  <si>
-    <t>Yang Wang</t>
-  </si>
-  <si>
     <t>William H. Wilson</t>
   </si>
   <si>
@@ -275,15 +211,6 @@
     <t>Raymond Wong</t>
   </si>
   <si>
-    <t>Hui Wu</t>
-  </si>
-  <si>
-    <t>Jingling Xue</t>
-  </si>
-  <si>
-    <t>Professor &amp; Associate HoS</t>
-  </si>
-  <si>
     <t>Ding Ye</t>
   </si>
   <si>
@@ -308,49 +235,7 @@
     <t>CSE Seminar Series - Roster</t>
   </si>
   <si>
-    <t xml:space="preserve">Qi Han </t>
-  </si>
-  <si>
-    <t>External</t>
-  </si>
-  <si>
-    <t>External (UTS)</t>
-  </si>
-  <si>
-    <t>Richard Xu</t>
-  </si>
-  <si>
-    <t>Dilip Sarkar</t>
-  </si>
-  <si>
-    <t>External (U. Miami)</t>
-  </si>
-  <si>
-    <t>Dr Michael Kasumovic</t>
-  </si>
-  <si>
-    <t>UNSW</t>
-  </si>
-  <si>
-    <t>Oliver Bown</t>
-  </si>
-  <si>
-    <t>UNSW Art &amp; Design</t>
-  </si>
-  <si>
     <t>ON FRIDAY DUE TO K17_113 AVAIL.</t>
-  </si>
-  <si>
-    <t>Jake Chandler</t>
-  </si>
-  <si>
-    <t>La Trobe University</t>
-  </si>
-  <si>
-    <t>Neal Patwari</t>
-  </si>
-  <si>
-    <t>Associate Professor, the University of Utah</t>
   </si>
   <si>
     <t>ON  FRIDAY</t>
@@ -363,7 +248,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -437,27 +322,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <u/>
-      <sz val="14"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -512,7 +376,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -522,12 +386,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -897,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -910,29 +768,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="A1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4">
         <v>42579</v>
@@ -964,10 +822,10 @@
     </row>
     <row r="6" spans="1:7" ht="19">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4">
         <f>C5+7</f>
@@ -976,16 +834,16 @@
     </row>
     <row r="7" spans="1:7" ht="19">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4">
         <v>42608</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="19">
@@ -1001,10 +859,10 @@
     </row>
     <row r="9" spans="1:7" ht="19">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" ref="C9:C17" si="0">C8+7</f>
@@ -1013,10 +871,10 @@
     </row>
     <row r="10" spans="1:7" ht="19">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
@@ -1040,7 +898,7 @@
     </row>
     <row r="12" spans="1:7" ht="19">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
@@ -1052,7 +910,7 @@
     </row>
     <row r="13" spans="1:7" ht="19">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
@@ -1064,10 +922,10 @@
     </row>
     <row r="14" spans="1:7" ht="19">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
@@ -1076,10 +934,10 @@
     </row>
     <row r="15" spans="1:7" ht="19">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
@@ -1088,10 +946,10 @@
     </row>
     <row r="16" spans="1:7" ht="19">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
@@ -1100,7 +958,7 @@
     </row>
     <row r="17" spans="1:4" ht="19">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
@@ -1112,24 +970,24 @@
     </row>
     <row r="18" spans="1:4" ht="19">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="4">
         <v>42671</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="19">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4">
         <v>42677</v>
@@ -1137,10 +995,10 @@
     </row>
     <row r="20" spans="1:4" ht="19">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" ref="C20:C35" si="1">C19+7</f>
@@ -1149,7 +1007,7 @@
     </row>
     <row r="21" spans="1:4" ht="19">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>5</v>
@@ -1161,10 +1019,10 @@
     </row>
     <row r="22" spans="1:4" ht="19">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
@@ -1173,10 +1031,10 @@
     </row>
     <row r="23" spans="1:4" ht="19">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
@@ -1185,7 +1043,7 @@
     </row>
     <row r="24" spans="1:4" ht="19">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>7</v>
@@ -1209,10 +1067,10 @@
     </row>
     <row r="26" spans="1:4" ht="19">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
@@ -1221,7 +1079,7 @@
     </row>
     <row r="27" spans="1:4" ht="19">
       <c r="A27" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>14</v>
@@ -1233,10 +1091,10 @@
     </row>
     <row r="28" spans="1:4" ht="19">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
@@ -1245,10 +1103,10 @@
     </row>
     <row r="29" spans="1:4" ht="19">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
@@ -1257,7 +1115,7 @@
     </row>
     <row r="30" spans="1:4" ht="19">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>5</v>
@@ -1269,7 +1127,7 @@
     </row>
     <row r="31" spans="1:4" ht="19">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>1</v>
@@ -1305,10 +1163,10 @@
     </row>
     <row r="34" spans="1:3" ht="19">
       <c r="A34" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
@@ -1329,10 +1187,10 @@
     </row>
     <row r="36" spans="1:3" ht="19">
       <c r="A36" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C36" s="4">
         <v>42754</v>
@@ -1340,10 +1198,10 @@
     </row>
     <row r="37" spans="1:3" ht="19">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C37" s="4">
         <f>C36+7</f>
@@ -1352,7 +1210,7 @@
     </row>
     <row r="38" spans="1:3" ht="19">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>14</v>
@@ -1376,10 +1234,10 @@
     </row>
     <row r="40" spans="1:3" ht="19">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="2"/>
@@ -1388,10 +1246,10 @@
     </row>
     <row r="41" spans="1:3" ht="19">
       <c r="A41" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="2"/>
@@ -1400,7 +1258,7 @@
     </row>
     <row r="42" spans="1:3" ht="19">
       <c r="A42" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>1</v>
@@ -1412,10 +1270,10 @@
     </row>
     <row r="43" spans="1:3" ht="19">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="2"/>
@@ -1424,7 +1282,7 @@
     </row>
     <row r="44" spans="1:3" ht="19">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>14</v>
@@ -1436,7 +1294,7 @@
     </row>
     <row r="45" spans="1:3" ht="19">
       <c r="A45" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>1</v>
@@ -1448,10 +1306,10 @@
     </row>
     <row r="46" spans="1:3" ht="19">
       <c r="A46" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="2"/>
@@ -1460,10 +1318,10 @@
     </row>
     <row r="47" spans="1:3" ht="19">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="2"/>
@@ -1472,7 +1330,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="2"/>
@@ -1537,386 +1395,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="4">
-        <v>42306</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4">
-        <f>C1+7</f>
-        <v>42313</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="4">
-        <f>C2+7</f>
-        <v>42320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4">
-        <f>C3+7</f>
-        <v>42327</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4">
-        <f>C4+7</f>
-        <v>42334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4">
-        <v>42404</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="4">
-        <f>C6+7</f>
-        <v>42411</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" ht="19">
-      <c r="A8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="8">
-        <f>C7+7</f>
-        <v>42418</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4">
-        <f>C8+7</f>
-        <v>42425</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4">
-        <f>C9+7</f>
-        <v>42432</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="4">
-        <f>C10+7</f>
-        <v>42439</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" s="4">
-        <v>42446</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <f>C12+7</f>
-        <v>42453</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A14" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="4">
-        <f>C13+7</f>
-        <v>42460</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4">
-        <v>42467</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4">
-        <f>C15+7</f>
-        <v>42474</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4">
-        <f>C16+7</f>
-        <v>42481</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="4">
-        <v>42488</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" ref="C19:C27" si="0">C18+7</f>
-        <v>42495</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="8">
-        <f t="shared" si="0"/>
-        <v>42502</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A21" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="8">
-        <f t="shared" si="0"/>
-        <v>42509</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="0"/>
-        <v>42516</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A23" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="8">
-        <f t="shared" si="0"/>
-        <v>42523</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="0"/>
-        <v>42530</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="4">
-        <f t="shared" si="0"/>
-        <v>42537</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="4">
-        <f t="shared" si="0"/>
-        <v>42544</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A27" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="8">
-        <f t="shared" si="0"/>
-        <v>42551</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C28" s="4">
-        <v>42558</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="19">
-      <c r="A29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="4">
-        <f>C28+7</f>
-        <v>42565</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A24" r:id="rId4"/>
-    <hyperlink ref="A29" r:id="rId5"/>
-    <hyperlink ref="A13" r:id="rId6"/>
-    <hyperlink ref="A20" r:id="rId7"/>
-    <hyperlink ref="A17" r:id="rId8"/>
-    <hyperlink ref="A23" r:id="rId9"/>
-    <hyperlink ref="A16" r:id="rId10"/>
-    <hyperlink ref="A4" r:id="rId11"/>
-    <hyperlink ref="A22" r:id="rId12"/>
-    <hyperlink ref="A5" r:id="rId13"/>
-    <hyperlink ref="A6" r:id="rId14"/>
-    <hyperlink ref="A8" r:id="rId15"/>
-    <hyperlink ref="A7" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A27" r:id="rId19"/>
-    <hyperlink ref="A25" r:id="rId20"/>
-    <hyperlink ref="A26" r:id="rId21"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>